<commit_message>
fix: correct accepted list entry
</commit_message>
<xml_diff>
--- a/data/_accepted.xlsx
+++ b/data/_accepted.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\icmc-website\src\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\icmc-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA47B636-FE3C-4618-B3DE-8BCE79B0B25C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2285A11-44DC-4766-A3F2-C03D95F0EFCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -672,10 +672,6 @@
 Huy Nguyen-Quoc</t>
   </si>
   <si>
-    <t>Ho Chi Minh City Open University, Malaysia
-Ho Chi Minh City Open University, Malaysia</t>
-  </si>
-  <si>
     <t>Satyam Omar
 Sahadeo Padhye
 Dhananjoy Dey</t>
@@ -986,6 +982,10 @@
     <t>Xavier School of Computer Science and Engineering, India
 University of Tromsø¸, Norway
 Jadavpur University, India</t>
+  </si>
+  <si>
+    <t>Ho Chi Minh City Open University, Vietnam
+Ho Chi Minh City Open University, Vietnam</t>
   </si>
 </sst>
 </file>
@@ -1088,17 +1088,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1321,8 +1321,8 @@
   </sheetPr>
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1336,28 +1336,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1505,7 +1505,7 @@
         <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>98</v>
@@ -1579,7 +1579,7 @@
         <v>107</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -1590,13 +1590,13 @@
         <v>68</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>226</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
@@ -1692,7 +1692,7 @@
         <v>93</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>114</v>
@@ -1749,7 +1749,7 @@
         <v>121</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2055,7 +2055,7 @@
         <v>152</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2086,7 +2086,7 @@
         <v>46</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>155</v>
@@ -2208,7 +2208,7 @@
         <v>169</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2225,7 +2225,7 @@
         <v>170</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>171</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2239,10 +2239,10 @@
         <v>54</v>
       </c>
       <c r="D54" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2256,10 +2256,10 @@
         <v>55</v>
       </c>
       <c r="D55" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2273,7 +2273,7 @@
         <v>56</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>160</v>
@@ -2287,13 +2287,13 @@
         <v>216</v>
       </c>
       <c r="C57" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="E57" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2307,10 +2307,10 @@
         <v>57</v>
       </c>
       <c r="D58" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2324,10 +2324,10 @@
         <v>58</v>
       </c>
       <c r="D59" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="67.5" x14ac:dyDescent="0.2">
@@ -2341,10 +2341,10 @@
         <v>59</v>
       </c>
       <c r="D60" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2358,10 +2358,10 @@
         <v>60</v>
       </c>
       <c r="D61" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2375,10 +2375,10 @@
         <v>61</v>
       </c>
       <c r="D62" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2392,10 +2392,10 @@
         <v>62</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2409,10 +2409,10 @@
         <v>63</v>
       </c>
       <c r="D64" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2426,10 +2426,10 @@
         <v>64</v>
       </c>
       <c r="D65" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2443,10 +2443,10 @@
         <v>65</v>
       </c>
       <c r="D66" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2460,10 +2460,10 @@
         <v>66</v>
       </c>
       <c r="D67" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2477,10 +2477,10 @@
         <v>67</v>
       </c>
       <c r="D68" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2494,7 +2494,7 @@
         <v>68</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>149</v>
@@ -2508,13 +2508,13 @@
         <v>320</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D70" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2528,10 +2528,10 @@
         <v>69</v>
       </c>
       <c r="D71" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2545,10 +2545,10 @@
         <v>70</v>
       </c>
       <c r="D72" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E72" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2562,10 +2562,10 @@
         <v>71</v>
       </c>
       <c r="D73" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E73" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2579,10 +2579,10 @@
         <v>72</v>
       </c>
       <c r="D74" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2596,10 +2596,10 @@
         <v>73</v>
       </c>
       <c r="D75" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E75" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2613,7 +2613,7 @@
         <v>74</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>149</v>
@@ -2630,10 +2630,10 @@
         <v>75</v>
       </c>
       <c r="D77" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E77" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2647,10 +2647,10 @@
         <v>76</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2664,10 +2664,10 @@
         <v>77</v>
       </c>
       <c r="D79" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E79" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2678,13 +2678,13 @@
         <v>361</v>
       </c>
       <c r="C80" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D80" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="E80" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2698,20 +2698,20 @@
         <v>78</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="10" t="s">
+      <c r="A82" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
     </row>
     <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E83" s="2"/>

</xml_diff>